<commit_message>
reading and posting entities to the database implemented
</commit_message>
<xml_diff>
--- a/resources/Vehicle-Load_data.xlsx
+++ b/resources/Vehicle-Load_data.xlsx
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Onhold</t>
   </si>
   <si>
-    <t xml:space="preserve">Diesel</t>
+    <t xml:space="preserve">Gasoline</t>
   </si>
   <si>
     <t xml:space="preserve">ABC1524</t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">Mini Van</t>
   </si>
   <si>
-    <t xml:space="preserve">Locker</t>
+    <t xml:space="preserve">Trailer</t>
   </si>
 </sst>
 </file>
@@ -136,7 +136,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -176,11 +176,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -224,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,10 +258,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -297,14 +288,14 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="K2:K5 D2"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
@@ -491,7 +482,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:K5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,11 +492,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="5" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="5" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="8.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="5" width="11.54"/>
   </cols>
   <sheetData>
@@ -560,20 +551,20 @@
       <c r="E2" s="5" t="n">
         <v>5890</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="F2" s="5" t="n">
         <v>2350</v>
       </c>
-      <c r="G2" s="10" t="n">
+      <c r="G2" s="5" t="n">
         <v>2360</v>
       </c>
-      <c r="I2" s="11" t="n">
+      <c r="I2" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="11" t="n">
+      <c r="K2" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -585,7 +576,7 @@
       <c r="B3" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="C3" s="11" t="n">
         <v>600</v>
       </c>
       <c r="D3" s="5" t="n">
@@ -594,20 +585,20 @@
       <c r="E3" s="5" t="n">
         <v>3246</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="5" t="n">
         <v>2350</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="5" t="n">
         <v>2360</v>
       </c>
-      <c r="I3" s="11" t="n">
+      <c r="I3" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="11" t="n">
+      <c r="K3" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -619,7 +610,7 @@
       <c r="B4" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="11" t="n">
         <v>10</v>
       </c>
       <c r="D4" s="5" t="n">
@@ -634,14 +625,14 @@
       <c r="G4" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="I4" s="11" t="n">
+      <c r="I4" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="11" t="n">
+      <c r="K4" s="10" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -653,7 +644,7 @@
       <c r="B5" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="11" t="n">
         <v>10</v>
       </c>
       <c r="D5" s="5" t="n">
@@ -668,23 +659,23 @@
       <c r="G5" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="I5" s="11" t="n">
+      <c r="I5" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="11" t="n">
+      <c r="K5" s="10" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="12"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="12"/>
+      <c r="C7" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>